<commit_message>
Update DB Attributes to change FLOAT to DECIMAL
The FLOAT data type does not accept (p,s) as I initially though so changed this to DECIMAL
</commit_message>
<xml_diff>
--- a/DB ATTRIBUTES.xlsx
+++ b/DB ATTRIBUTES.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephanie\Documents\Bow Valley Tech Initiative\Industry Project\My Version\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephanie\Documents\GitHub\BVC_IndProject_Municipal_Election_Analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7661307-42D7-40F7-AE18-A7A1CC423519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299C9C74-983C-4A13-8D35-9F4867D2E5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="0" windowWidth="11640" windowHeight="17415" xr2:uid="{E93B2AC0-2CA5-4D8A-A975-600A3DD0DDC6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E93B2AC0-2CA5-4D8A-A975-600A3DD0DDC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -204,9 +204,6 @@
     <t>VARCHAR(7)</t>
   </si>
   <si>
-    <t>FLOAT(3,2)</t>
-  </si>
-  <si>
     <t>NVARCHAR(50)</t>
   </si>
   <si>
@@ -247,6 +244,9 @@
   </si>
   <si>
     <t>Mayor, Councillor, Public School Trustee, Separate School Trustee</t>
+  </si>
+  <si>
+    <t>DECIMAL(3,2)</t>
   </si>
 </sst>
 </file>
@@ -841,7 +841,7 @@
         <v>44</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>43</v>
@@ -862,10 +862,10 @@
         <v>49</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -873,7 +873,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="35"/>
     </row>
@@ -1089,10 +1089,10 @@
         <v>49</v>
       </c>
       <c r="D27" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="24" t="s">
         <v>64</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -1100,7 +1100,7 @@
         <v>25</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D28" s="37"/>
     </row>
@@ -1118,7 +1118,7 @@
         <v>54</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -1126,7 +1126,7 @@
         <v>27</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D30" s="38"/>
     </row>
@@ -1144,7 +1144,7 @@
         <v>29</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="D32" s="38"/>
     </row>
@@ -1159,10 +1159,10 @@
         <v>49</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E33" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -1173,7 +1173,7 @@
         <v>50</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -1187,10 +1187,10 @@
         <v>49</v>
       </c>
       <c r="D35" s="40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -1201,7 +1201,7 @@
         <v>50</v>
       </c>
       <c r="D36" s="40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -1215,10 +1215,10 @@
         <v>49</v>
       </c>
       <c r="D37" s="41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="30" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1229,7 +1229,7 @@
         <v>51</v>
       </c>
       <c r="D38" s="41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -1243,10 +1243,10 @@
         <v>49</v>
       </c>
       <c r="D39" s="42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
         <v>55</v>
       </c>
       <c r="D40" s="42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
@@ -1271,10 +1271,10 @@
         <v>49</v>
       </c>
       <c r="D41" s="43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>